<commit_message>
- PhotoMixer 0.8beta release 2011-12-04
</commit_message>
<xml_diff>
--- a/Doc/PhotoMixer.xlsx
+++ b/Doc/PhotoMixer.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>TODOS</t>
   </si>
@@ -37,6 +37,21 @@
   </si>
   <si>
     <t>Testing - prepare sets for different scenarios, process, and compare with expected results</t>
+  </si>
+  <si>
+    <t>RefSource selection doesný need to be on output page, put it to Source page as checkbox or something (only needed for RefSync mode - no need to be on outpt page that is for all)</t>
+  </si>
+  <si>
+    <t>Make Source name edit focused control when new Source is created</t>
+  </si>
+  <si>
+    <t>Custom naming patterns - as advanced option</t>
+  </si>
+  <si>
+    <t>Add seconds to default pattern - when adding additional prhotos to previously done mix there maybe overwrites since the counter starts at zero on additional mix</t>
+  </si>
+  <si>
+    <t>When Tool is executed go to output page to see the log</t>
   </si>
 </sst>
 </file>
@@ -397,10 +412,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -444,6 +459,31 @@
         <v>6</v>
       </c>
     </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -453,7 +493,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>

<commit_message>
- auto orientation by Exif (using NativeJpg for lossless JPEG transforms) - reworked tools UIs (using frames and dynamically created forms)
</commit_message>
<xml_diff>
--- a/Doc/PhotoMixer.xlsx
+++ b/Doc/PhotoMixer.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="26835" windowHeight="15135"/>
+    <workbookView xWindow="480" yWindow="30" windowWidth="19455" windowHeight="10680"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>TODOS</t>
   </si>
@@ -52,13 +52,22 @@
   </si>
   <si>
     <t>When Tool is executed go to output page to see the log</t>
+  </si>
+  <si>
+    <t>Auto-orient by EXIF + reset exif orient tag (make sure other metadata is left intact)</t>
+  </si>
+  <si>
+    <t>must have 4 modes = one is "do not modify - just renaming and adding to output mix"</t>
+  </si>
+  <si>
+    <t>Add credits for CCR-Exif and NativeJpg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -76,13 +85,35 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -103,15 +134,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
+    <cellStyle name="Explanatory Text" xfId="3" builtinId="53"/>
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -412,10 +449,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -445,43 +482,58 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>4</v>
+      <c r="B6" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- more UI stuff moved to frames - UI for custom ref. master sources
</commit_message>
<xml_diff>
--- a/Doc/PhotoMixer.xlsx
+++ b/Doc/PhotoMixer.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>TODOS</t>
   </si>
@@ -61,6 +61,12 @@
   </si>
   <si>
     <t>Add credits for CCR-Exif and NativeJpg</t>
+  </si>
+  <si>
+    <t>Advanced source sync (for Japan trip) - for when there is no ref photo shared by all sources, but only e.g. A-B + B-C + B-D + C-E</t>
+  </si>
+  <si>
+    <t>"View" button for ref. photos so that user can quickly check if the right photo is selected (just open associated program is ok)</t>
   </si>
 </sst>
 </file>
@@ -449,10 +455,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -534,6 +540,16 @@
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>